<commit_message>
I only manually modified the Teacher classes.
</commit_message>
<xml_diff>
--- a/Prototype/Prototype/Teachers/ElementaryTeachers.xlsx
+++ b/Prototype/Prototype/Teachers/ElementaryTeachers.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/derekbailey/Projects/Shelbatron1000/LVS_App.git/Prototype/Prototype/Teachers/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="12220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>Elementary</t>
   </si>
@@ -44,21 +44,9 @@
     <t>karlaaa@leeschools.net</t>
   </si>
   <si>
-    <t>239-281-4712</t>
-  </si>
-  <si>
-    <t>Thursday 9 a.m. to 4 p.m.</t>
-  </si>
-  <si>
     <t>monicasd@leeschools.net</t>
   </si>
   <si>
-    <t>239-822-0318</t>
-  </si>
-  <si>
-    <t>Wed 1-3 Thur 10-12</t>
-  </si>
-  <si>
     <t>(239) 357-7602</t>
   </si>
   <si>
@@ -68,26 +56,101 @@
     <t>Please make an appointment</t>
   </si>
   <si>
-    <t>Monday- Friday 8AM-8PM</t>
-  </si>
-  <si>
-    <t>239- 823-8065</t>
-  </si>
-  <si>
     <t>AnaleeEM@leeschools.net</t>
+  </si>
+  <si>
+    <t>(239) 281-4712</t>
+  </si>
+  <si>
+    <t>Thurs 9am-4pm</t>
+  </si>
+  <si>
+    <t>(239) 822-0318</t>
+  </si>
+  <si>
+    <t>Wed 1pm-3pm, Thur 10am-12pm</t>
+  </si>
+  <si>
+    <t>(239) 823-8065</t>
+  </si>
+  <si>
+    <t>Mon- Frid 8am-8pm</t>
+  </si>
+  <si>
+    <t>Secondary</t>
+  </si>
+  <si>
+    <t>Mr. Bruni</t>
+  </si>
+  <si>
+    <t>Jamesdb@leeschools.net</t>
+  </si>
+  <si>
+    <t>(239) 357-8038</t>
+  </si>
+  <si>
+    <t>Mon 9am-12pm</t>
+  </si>
+  <si>
+    <t>Mr. McKinley</t>
+  </si>
+  <si>
+    <t>edwardamck@leeschools.net</t>
+  </si>
+  <si>
+    <t>(239) 822-9725</t>
+  </si>
+  <si>
+    <t>Thur 3pm-4pm</t>
+  </si>
+  <si>
+    <t>Mrs. Ausman</t>
+  </si>
+  <si>
+    <t>MeaganMA@leeschools.net</t>
+  </si>
+  <si>
+    <t>(239) 823-2565</t>
+  </si>
+  <si>
+    <t>Mon-Fri 7am-8pm</t>
+  </si>
+  <si>
+    <t>Mrs. Brooks</t>
+  </si>
+  <si>
+    <t>brittanypb@leeschools.net</t>
+  </si>
+  <si>
+    <t>(239) 357-2709</t>
+  </si>
+  <si>
+    <t>Thur 1pm-4pm by Appointment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -110,9 +173,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,89 +491,157 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="27.140625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="12.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="27.1640625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="E3" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>14</v>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>